<commit_message>
Revising SHGC to 0.26 for parts 1 and 2 of study and updating results spreadsheet.
</commit_message>
<xml_diff>
--- a/NBC-tiered-code/solar-threshold-study/OS_models/NZEH_OS_peak_heat_cool.xlsx
+++ b/NBC-tiered-code/solar-threshold-study/OS_models/NZEH_OS_peak_heat_cool.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckirney\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckirney\projects\HTAP-projects\NBC-tiered-code\solar-threshold-study\OS_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -417,9 +417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -434,7 +432,7 @@
         <v>20</v>
       </c>
       <c r="E1">
-        <v>0.56999999999999995</v>
+        <v>0.26</v>
       </c>
       <c r="F1" t="s">
         <v>21</v>
@@ -485,16 +483,16 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>12.84</v>
+        <v>14.1</v>
       </c>
       <c r="C4">
-        <v>4.6900000000000004</v>
+        <v>2.15</v>
       </c>
       <c r="D4">
         <v>26.39</v>
       </c>
       <c r="E4">
-        <v>1.66</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -502,16 +500,16 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>12.84</v>
+        <v>14.1</v>
       </c>
       <c r="C5">
-        <v>4.6900000000000004</v>
+        <v>2.15</v>
       </c>
       <c r="D5">
         <v>26.39</v>
       </c>
       <c r="E5">
-        <v>1.66</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -519,16 +517,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>13.13</v>
+        <v>14.56</v>
       </c>
       <c r="C6">
-        <v>5.35</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D6">
         <v>27.64</v>
       </c>
       <c r="E6">
-        <v>1.89</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -536,16 +534,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>13.33</v>
+        <v>14.86</v>
       </c>
       <c r="C7">
-        <v>5.83</v>
+        <v>2.66</v>
       </c>
       <c r="D7">
         <v>28.48</v>
       </c>
       <c r="E7">
-        <v>2.0499999999999998</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -553,32 +551,32 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>11.89</v>
+        <v>13.16</v>
       </c>
       <c r="C9">
-        <v>2.2799999999999998</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D9">
         <v>24.64</v>
       </c>
       <c r="E9">
-        <v>0.84</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F9">
         <f t="shared" ref="F9:G11" si="0">B9-B4</f>
-        <v>-0.94999999999999929</v>
+        <v>-0.9399999999999995</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>-2.4100000000000006</v>
+        <v>-1.01</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" ref="H9:I11" si="1">F9/B4</f>
-        <v>-7.3987538940809908E-2</v>
+        <v>-6.6666666666666638E-2</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>-0.51385927505330498</v>
+        <v>-0.46976744186046515</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" ref="J9:K11" si="2">(D9-D4)/D4</f>
@@ -586,7 +584,7 @@
       </c>
       <c r="K9" s="2">
         <f t="shared" si="2"/>
-        <v>-0.49397590361445781</v>
+        <v>-0.40217391304347822</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -594,32 +592,32 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>11.16</v>
+        <v>12.33</v>
       </c>
       <c r="C10">
-        <v>1.69</v>
+        <v>0.93</v>
       </c>
       <c r="D10">
         <v>22.79</v>
       </c>
       <c r="E10">
-        <v>0.63</v>
+        <v>0.45</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>-1.6799999999999997</v>
+        <v>-1.7699999999999996</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
-        <v>-3.0000000000000004</v>
+        <v>-1.2199999999999998</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>-0.13084112149532709</v>
+        <v>-0.12553191489361698</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>-0.63965884861407252</v>
+        <v>-0.56744186046511613</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="2"/>
@@ -627,7 +625,7 @@
       </c>
       <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>-0.62048192771084332</v>
+        <v>-0.51086956521739135</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -635,32 +633,32 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>12.4</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>3.2</v>
+        <v>1.5</v>
       </c>
       <c r="D11">
         <v>27.41</v>
       </c>
       <c r="E11">
-        <v>1.1399999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>-0.73000000000000043</v>
+        <v>-0.5600000000000005</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>-2.1499999999999995</v>
+        <v>-0.95000000000000018</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>-5.5597867479055624E-2</v>
+        <v>-3.8461538461538491E-2</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>-0.40186915887850461</v>
+        <v>-0.38775510204081637</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="2"/>
@@ -668,7 +666,7 @@
       </c>
       <c r="K11" s="2">
         <f t="shared" si="2"/>
-        <v>-0.39682539682539686</v>
+        <v>-0.33653846153846162</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -676,32 +674,32 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>12.93</v>
+        <v>14.65</v>
       </c>
       <c r="C12">
-        <v>3.77</v>
+        <v>1.74</v>
       </c>
       <c r="D12">
         <v>29.42</v>
       </c>
       <c r="E12">
-        <v>1.34</v>
+        <v>0.8</v>
       </c>
       <c r="F12">
         <f t="shared" ref="F12" si="3">B12-B7</f>
-        <v>-0.40000000000000036</v>
+        <v>-0.20999999999999908</v>
       </c>
       <c r="G12">
         <f t="shared" ref="G12" si="4">C12-C7</f>
-        <v>-2.06</v>
+        <v>-0.92000000000000015</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" ref="H12" si="5">F12/B7</f>
-        <v>-3.0007501875468894E-2</v>
+        <v>-1.4131897711978404E-2</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" ref="I12" si="6">G12/C7</f>
-        <v>-0.35334476843910806</v>
+        <v>-0.34586466165413537</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" ref="J12" si="7">(D12-D7)/D7</f>
@@ -709,7 +707,7 @@
       </c>
       <c r="K12" s="2">
         <f t="shared" ref="K12" si="8">(E12-E7)/E7</f>
-        <v>-0.34634146341463407</v>
+        <v>-0.28571428571428575</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -754,16 +752,16 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>12.84</v>
+        <v>14.1</v>
       </c>
       <c r="C16">
-        <v>4.6900000000000004</v>
+        <v>2.15</v>
       </c>
       <c r="D16">
         <v>26.39</v>
       </c>
       <c r="E16">
-        <v>1.66</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -771,16 +769,16 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>12.84</v>
+        <v>14.1</v>
       </c>
       <c r="C17">
-        <v>4.6900000000000004</v>
+        <v>2.15</v>
       </c>
       <c r="D17">
         <v>26.39</v>
       </c>
       <c r="E17">
-        <v>1.66</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -788,16 +786,16 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <v>13.13</v>
+        <v>14.56</v>
       </c>
       <c r="C18">
-        <v>5.35</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D18">
         <v>27.64</v>
       </c>
       <c r="E18">
-        <v>1.89</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -805,16 +803,16 @@
         <v>10</v>
       </c>
       <c r="B19">
-        <v>13.33</v>
+        <v>14.86</v>
       </c>
       <c r="C19">
-        <v>5.83</v>
+        <v>2.66</v>
       </c>
       <c r="D19">
         <v>28.48</v>
       </c>
       <c r="E19">
-        <v>2.0499999999999998</v>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -822,32 +820,32 @@
         <v>3</v>
       </c>
       <c r="B21">
-        <v>12.9</v>
+        <v>13.68</v>
       </c>
       <c r="C21">
-        <v>4.2</v>
+        <v>1.97</v>
       </c>
       <c r="D21">
         <v>24.64</v>
       </c>
       <c r="E21">
-        <v>1.89</v>
+        <v>1.02</v>
       </c>
       <c r="F21">
         <f t="shared" ref="F21:F24" si="9">B21-B16</f>
-        <v>6.0000000000000497E-2</v>
+        <v>-0.41999999999999993</v>
       </c>
       <c r="G21">
         <f t="shared" ref="G21:G24" si="10">C21-C16</f>
-        <v>-0.49000000000000021</v>
+        <v>-0.17999999999999994</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" ref="H21:H24" si="11">F21/B16</f>
-        <v>4.6728971962617209E-3</v>
+        <v>-2.9787234042553186E-2</v>
       </c>
       <c r="I21" s="1">
         <f t="shared" ref="I21:I24" si="12">G21/C16</f>
-        <v>-0.10447761194029855</v>
+        <v>-8.3720930232558111E-2</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" ref="J21:J24" si="13">(D21-D16)/D16</f>
@@ -855,7 +853,7 @@
       </c>
       <c r="K21" s="2">
         <f t="shared" ref="K21:K24" si="14">(E21-E16)/E16</f>
-        <v>0.13855421686746988</v>
+        <v>0.10869565217391301</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -863,32 +861,32 @@
         <v>8</v>
       </c>
       <c r="B22">
-        <v>12.29</v>
+        <v>12.89</v>
       </c>
       <c r="C22">
-        <v>2.84</v>
+        <v>1.42</v>
       </c>
       <c r="D22">
         <v>22.82</v>
       </c>
       <c r="E22">
-        <v>1.72</v>
+        <v>0.93</v>
       </c>
       <c r="F22">
         <f t="shared" si="9"/>
-        <v>-0.55000000000000071</v>
+        <v>-1.2099999999999991</v>
       </c>
       <c r="G22">
         <f t="shared" si="10"/>
-        <v>-1.8500000000000005</v>
+        <v>-0.73</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="11"/>
-        <v>-4.2834890965732141E-2</v>
+        <v>-8.5815602836879376E-2</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" si="12"/>
-        <v>-0.3944562899786781</v>
+        <v>-0.33953488372093021</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="13"/>
@@ -896,7 +894,7 @@
       </c>
       <c r="K22" s="2">
         <f t="shared" si="14"/>
-        <v>3.6144578313253045E-2</v>
+        <v>1.0869565217391313E-2</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -904,32 +902,32 @@
         <v>11</v>
       </c>
       <c r="B23">
-        <v>13.62</v>
+        <v>14.77</v>
       </c>
       <c r="C23">
-        <v>6.01</v>
+        <v>2.77</v>
       </c>
       <c r="D23">
         <v>27.42</v>
       </c>
       <c r="E23">
-        <v>2.76</v>
+        <v>1.44</v>
       </c>
       <c r="F23">
         <f t="shared" si="9"/>
-        <v>0.48999999999999844</v>
+        <v>0.20999999999999908</v>
       </c>
       <c r="G23">
         <f t="shared" si="10"/>
-        <v>0.66000000000000014</v>
+        <v>0.31999999999999984</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="11"/>
-        <v>3.7319116527037198E-2</v>
+        <v>1.442307692307686E-2</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="12"/>
-        <v>0.12336448598130845</v>
+        <v>0.13061224489795911</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="13"/>
@@ -937,7 +935,7 @@
       </c>
       <c r="K23" s="2">
         <f t="shared" si="14"/>
-        <v>0.46031746031746029</v>
+        <v>0.38461538461538453</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -945,32 +943,32 @@
         <v>12</v>
       </c>
       <c r="B24">
-        <v>14.25</v>
+        <v>15.59</v>
       </c>
       <c r="C24">
-        <v>7.2</v>
+        <v>3.31</v>
       </c>
       <c r="D24">
         <v>29.44</v>
       </c>
       <c r="E24">
-        <v>3.36</v>
+        <v>1.74</v>
       </c>
       <c r="F24">
         <f t="shared" si="9"/>
-        <v>0.91999999999999993</v>
+        <v>0.73000000000000043</v>
       </c>
       <c r="G24">
         <f t="shared" si="10"/>
-        <v>1.37</v>
+        <v>0.64999999999999991</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="11"/>
-        <v>6.9017254313578386E-2</v>
+        <v>4.9125168236877556E-2</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="12"/>
-        <v>0.23499142367066897</v>
+        <v>0.24436090225563906</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="13"/>
@@ -978,7 +976,7 @@
       </c>
       <c r="K24" s="2">
         <f t="shared" si="14"/>
-        <v>0.63902439024390256</v>
+        <v>0.55357142857142838</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1056,19 +1054,19 @@
       </c>
       <c r="F29">
         <f>B29-$B$4</f>
-        <v>-0.51999999999999957</v>
+        <v>-1.7799999999999994</v>
       </c>
       <c r="G29">
         <f>C29-$C$4</f>
-        <v>-2.6700000000000004</v>
+        <v>-0.12999999999999989</v>
       </c>
       <c r="H29" s="1">
         <f>F29/$B$4</f>
-        <v>-4.0498442367601216E-2</v>
+        <v>-0.12624113475177301</v>
       </c>
       <c r="I29" s="1">
         <f>G29/$C$4</f>
-        <v>-0.56929637526652455</v>
+        <v>-6.0465116279069718E-2</v>
       </c>
       <c r="J29" s="1">
         <f>(D29-$D$4)/$D$4</f>
@@ -1076,7 +1074,7 @@
       </c>
       <c r="K29" s="2">
         <f>(E29-$E$4)/$E$4</f>
-        <v>-0.52409638554216864</v>
+        <v>-0.14130434782608695</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1097,19 +1095,19 @@
       </c>
       <c r="F30">
         <f>B30-$B$5</f>
-        <v>-1.3200000000000003</v>
+        <v>-2.58</v>
       </c>
       <c r="G30">
         <f>C30-$C$5</f>
-        <v>-3.1800000000000006</v>
+        <v>-0.6399999999999999</v>
       </c>
       <c r="H30" s="1">
         <f>F30/$B$5</f>
-        <v>-0.10280373831775703</v>
+        <v>-0.18297872340425533</v>
       </c>
       <c r="I30" s="1">
         <f>G30/$C$5</f>
-        <v>-0.67803837953091695</v>
+        <v>-0.2976744186046511</v>
       </c>
       <c r="J30" s="1">
         <f>(D30-$D$5)/$D$5</f>
@@ -1117,7 +1115,7 @@
       </c>
       <c r="K30" s="2">
         <f>(E30-$E$5)/$E$5</f>
-        <v>-0.64457831325301196</v>
+        <v>-0.35869565217391308</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1138,19 +1136,19 @@
       </c>
       <c r="F31">
         <f>B31-$B$6</f>
-        <v>-0.19000000000000128</v>
+        <v>-1.620000000000001</v>
       </c>
       <c r="G31">
         <f>C31-$C$6</f>
-        <v>-2.5199999999999996</v>
+        <v>0.37999999999999989</v>
       </c>
       <c r="H31" s="1">
         <f>F31/$B$6</f>
-        <v>-1.4470677837014567E-2</v>
+        <v>-0.11126373626373633</v>
       </c>
       <c r="I31" s="1">
         <f>G31/$C$6</f>
-        <v>-0.4710280373831775</v>
+        <v>0.15510204081632648</v>
       </c>
       <c r="J31" s="1">
         <f>(D31-$D$6)/$D$6</f>
@@ -1158,7 +1156,7 @@
       </c>
       <c r="K31" s="2">
         <f>(E31-$E$6)/$E$6</f>
-        <v>-0.43915343915343907</v>
+        <v>1.9230769230769246E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1179,19 +1177,19 @@
       </c>
       <c r="F32">
         <f>B32-$B$7</f>
-        <v>0.19999999999999929</v>
+        <v>-1.33</v>
       </c>
       <c r="G32">
         <f>C32-$C$7</f>
-        <v>-2.4900000000000002</v>
+        <v>0.67999999999999972</v>
       </c>
       <c r="H32" s="1">
         <f>F32/$B$7</f>
-        <v>1.5003750937734379E-2</v>
+        <v>-8.9502018842530284E-2</v>
       </c>
       <c r="I32" s="1">
         <f>G32/$C$7</f>
-        <v>-0.42710120068610635</v>
+        <v>0.25563909774436078</v>
       </c>
       <c r="J32" s="1">
         <f>(D32-$D$7)/$D$7</f>
@@ -1199,7 +1197,7 @@
       </c>
       <c r="K32" s="2">
         <f>(E32-$E$7)/$E$7</f>
-        <v>-0.39024390243902435</v>
+        <v>0.11607142857142846</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -1257,19 +1255,19 @@
       </c>
       <c r="F36">
         <f>B36-$B$4</f>
-        <v>0.40000000000000036</v>
+        <v>-0.85999999999999943</v>
       </c>
       <c r="G36">
         <f>C36-$C$4</f>
-        <v>-0.99000000000000021</v>
+        <v>1.5500000000000003</v>
       </c>
       <c r="H36" s="1">
         <f>F36/$B$4</f>
-        <v>3.1152647975077909E-2</v>
+        <v>-6.0992907801418403E-2</v>
       </c>
       <c r="I36" s="1">
         <f>G36/$C$4</f>
-        <v>-0.21108742004264394</v>
+        <v>0.72093023255813971</v>
       </c>
       <c r="J36" s="1">
         <f>(D36-$D$4)/$D$4</f>
@@ -1277,7 +1275,7 @@
       </c>
       <c r="K36" s="2">
         <f>(E36-$E$4)/$E$4</f>
-        <v>2.4096385542168697E-2</v>
+        <v>0.84782608695652162</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1298,19 +1296,19 @@
       </c>
       <c r="F37">
         <f>B37-$B$5</f>
-        <v>-0.30000000000000071</v>
+        <v>-1.5600000000000005</v>
       </c>
       <c r="G37">
         <f>C37-$C$5</f>
-        <v>-2.1800000000000006</v>
+        <v>0.35999999999999988</v>
       </c>
       <c r="H37" s="1">
         <f>F37/$B$5</f>
-        <v>-2.3364485981308466E-2</v>
+        <v>-0.11063829787234046</v>
       </c>
       <c r="I37" s="1">
         <f>G37/$C$5</f>
-        <v>-0.46481876332622613</v>
+        <v>0.16744186046511622</v>
       </c>
       <c r="J37" s="1">
         <f>(D37-$D$5)/$D$5</f>
@@ -1318,7 +1316,7 @@
       </c>
       <c r="K37" s="2">
         <f>(E37-$E$5)/$E$5</f>
-        <v>-7.2289156626505952E-2</v>
+        <v>0.67391304347826086</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1339,19 +1337,19 @@
       </c>
       <c r="F38">
         <f>B38-$B$6</f>
-        <v>0.98999999999999844</v>
+        <v>-0.44000000000000128</v>
       </c>
       <c r="G38">
         <f>C38-$C$6</f>
-        <v>-4.9999999999999822E-2</v>
+        <v>2.8499999999999996</v>
       </c>
       <c r="H38" s="1">
         <f>F38/$B$6</f>
-        <v>7.5399847677075277E-2</v>
+        <v>-3.0219780219780307E-2</v>
       </c>
       <c r="I38" s="1">
         <f>G38/$C$6</f>
-        <v>-9.3457943925233326E-3</v>
+        <v>1.1632653061224487</v>
       </c>
       <c r="J38" s="1">
         <f>(D38-$D$6)/$D$6</f>
@@ -1359,7 +1357,7 @@
       </c>
       <c r="K38" s="2">
         <f>(E38-$E$6)/$E$6</f>
-        <v>0.31216931216931221</v>
+        <v>1.3846153846153846</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1380,19 +1378,19 @@
       </c>
       <c r="F39">
         <f>B39-$B$7</f>
-        <v>1.5099999999999998</v>
+        <v>-1.9999999999999574E-2</v>
       </c>
       <c r="G39">
         <f>C39-$C$7</f>
-        <v>0.53000000000000025</v>
+        <v>3.7</v>
       </c>
       <c r="H39" s="1">
         <f>F39/$B$7</f>
-        <v>0.11327831957989495</v>
+        <v>-1.3458950201883967E-3</v>
       </c>
       <c r="I39" s="1">
         <f>G39/$C$7</f>
-        <v>9.0909090909090953E-2</v>
+        <v>1.3909774436090225</v>
       </c>
       <c r="J39" s="1">
         <f>(D39-$D$7)/$D$7</f>
@@ -1400,7 +1398,7 @@
       </c>
       <c r="K39" s="2">
         <f>(E39-$E$7)/$E$7</f>
-        <v>0.47317073170731722</v>
+        <v>1.6964285714285712</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -1478,19 +1476,19 @@
       </c>
       <c r="F44">
         <f>B44-$B$4</f>
-        <v>0.1899999999999995</v>
+        <v>-1.0700000000000003</v>
       </c>
       <c r="G44">
         <f>C44-$C$4</f>
-        <v>-3.5300000000000002</v>
+        <v>-0.99</v>
       </c>
       <c r="H44" s="1">
         <f>F44/$B$4</f>
-        <v>1.4797507788161956E-2</v>
+        <v>-7.5886524822695062E-2</v>
       </c>
       <c r="I44" s="1">
         <f>G44/$C$4</f>
-        <v>-0.75266524520255862</v>
+        <v>-0.46046511627906977</v>
       </c>
       <c r="J44" s="1">
         <f>(D44-$D$4)/$D$4</f>
@@ -1498,7 +1496,7 @@
       </c>
       <c r="K44" s="2">
         <f>(E44-$E$4)/$E$4</f>
-        <v>-0.66867469879518071</v>
+        <v>-0.40217391304347822</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -1519,19 +1517,19 @@
       </c>
       <c r="F45">
         <f>B45-$B$5</f>
-        <v>-0.59999999999999964</v>
+        <v>-1.8599999999999994</v>
       </c>
       <c r="G45">
         <f>C45-$C$5</f>
-        <v>-4.4000000000000004</v>
+        <v>-1.8599999999999999</v>
       </c>
       <c r="H45" s="1">
         <f>F45/$B$5</f>
-        <v>-4.6728971962616793E-2</v>
+        <v>-0.13191489361702124</v>
       </c>
       <c r="I45" s="1">
         <f>G45/$C$5</f>
-        <v>-0.93816631130063965</v>
+        <v>-0.8651162790697674</v>
       </c>
       <c r="J45" s="1">
         <f>(D45-$D$5)/$D$5</f>
@@ -1539,7 +1537,7 @@
       </c>
       <c r="K45" s="2">
         <f>(E45-$E$5)/$E$5</f>
-        <v>-0.72891566265060237</v>
+        <v>-0.51086956521739135</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -1560,19 +1558,19 @@
       </c>
       <c r="F46">
         <f>B46-$B$6</f>
-        <v>0.67999999999999972</v>
+        <v>-0.75</v>
       </c>
       <c r="G46">
         <f>C46-$C$6</f>
-        <v>-3.8199999999999994</v>
+        <v>-0.92000000000000015</v>
       </c>
       <c r="H46" s="1">
         <f>F46/$B$6</f>
-        <v>5.1789794364051768E-2</v>
+        <v>-5.1510989010989008E-2</v>
       </c>
       <c r="I46" s="1">
         <f>G46/$C$6</f>
-        <v>-0.71401869158878495</v>
+        <v>-0.37551020408163271</v>
       </c>
       <c r="J46" s="1">
         <f>(D46-$D$6)/$D$6</f>
@@ -1580,7 +1578,7 @@
       </c>
       <c r="K46" s="2">
         <f>(E46-$E$6)/$E$6</f>
-        <v>-0.62962962962962965</v>
+        <v>-0.32692307692307698</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -1601,19 +1599,19 @@
       </c>
       <c r="F47">
         <f>B47-$B$7</f>
-        <v>1.08</v>
+        <v>-0.44999999999999929</v>
       </c>
       <c r="G47">
         <f>C47-$C$7</f>
-        <v>-4.05</v>
+        <v>-0.88000000000000012</v>
       </c>
       <c r="H47" s="1">
         <f>F47/$B$7</f>
-        <v>8.102025506376595E-2</v>
+        <v>-3.0282637954239522E-2</v>
       </c>
       <c r="I47" s="1">
         <f>G47/$C$7</f>
-        <v>-0.69468267581475129</v>
+        <v>-0.33082706766917297</v>
       </c>
       <c r="J47" s="1">
         <f>(D47-$D$7)/$D$7</f>
@@ -1621,7 +1619,7 @@
       </c>
       <c r="K47" s="2">
         <f>(E47-$E$7)/$E$7</f>
-        <v>-0.6097560975609756</v>
+        <v>-0.28571428571428575</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -1679,19 +1677,19 @@
       </c>
       <c r="F51">
         <f>B51-$B$4</f>
-        <v>0.71000000000000085</v>
+        <v>-0.54999999999999893</v>
       </c>
       <c r="G51">
         <f>C51-$C$4</f>
-        <v>-2.7</v>
+        <v>-0.15999999999999992</v>
       </c>
       <c r="H51" s="1">
         <f>F51/$B$4</f>
-        <v>5.5295950155763308E-2</v>
+        <v>-3.9007092198581485E-2</v>
       </c>
       <c r="I51" s="1">
         <f>G51/$C$4</f>
-        <v>-0.57569296375266521</v>
+        <v>-7.4418604651162762E-2</v>
       </c>
       <c r="J51" s="1">
         <f>(D51-$D$4)/$D$4</f>
@@ -1699,7 +1697,7 @@
       </c>
       <c r="K51" s="2">
         <f>(E51-$E$4)/$E$4</f>
-        <v>-0.38554216867469876</v>
+        <v>0.10869565217391301</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -1720,19 +1718,19 @@
       </c>
       <c r="F52">
         <f>B52-$B$5</f>
-        <v>-2.9999999999999361E-2</v>
+        <v>-1.2899999999999991</v>
       </c>
       <c r="G52">
         <f>C52-$C$5</f>
-        <v>-3.2500000000000004</v>
+        <v>-0.71</v>
       </c>
       <c r="H52" s="1">
         <f>F52/$B$5</f>
-        <v>-2.3364485981307915E-3</v>
+        <v>-9.1489361702127597E-2</v>
       </c>
       <c r="I52" s="1">
         <f>G52/$C$5</f>
-        <v>-0.69296375266524524</v>
+        <v>-0.33023255813953489</v>
       </c>
       <c r="J52" s="1">
         <f>(D52-$D$5)/$D$5</f>
@@ -1740,7 +1738,7 @@
       </c>
       <c r="K52" s="2">
         <f>(E52-$E$5)/$E$5</f>
-        <v>-0.43975903614457823</v>
+        <v>1.0869565217391313E-2</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -1761,19 +1759,19 @@
       </c>
       <c r="F53">
         <f>B53-$B$6</f>
-        <v>1.4399999999999995</v>
+        <v>9.9999999999997868E-3</v>
       </c>
       <c r="G53">
         <f>C53-$C$6</f>
-        <v>-2.5399999999999996</v>
+        <v>0.35999999999999988</v>
       </c>
       <c r="H53" s="1">
         <f>F53/$B$6</f>
-        <v>0.10967250571210962</v>
+        <v>6.8681318681317212E-4</v>
       </c>
       <c r="I53" s="1">
         <f>G53/$C$6</f>
-        <v>-0.47476635514018689</v>
+        <v>0.14693877551020401</v>
       </c>
       <c r="J53" s="1">
         <f>(D53-$D$6)/$D$6</f>
@@ -1781,7 +1779,7 @@
       </c>
       <c r="K53" s="2">
         <f>(E53-$E$6)/$E$6</f>
-        <v>-0.23280423280423279</v>
+        <v>0.39423076923076916</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -1802,19 +1800,19 @@
       </c>
       <c r="F54">
         <f>B54-$B$7</f>
-        <v>2.0199999999999996</v>
+        <v>0.49000000000000021</v>
       </c>
       <c r="G54">
         <f>C54-$C$7</f>
-        <v>-2.4700000000000002</v>
+        <v>0.69999999999999973</v>
       </c>
       <c r="H54" s="1">
         <f>F54/$B$7</f>
-        <v>0.15153788447111774</v>
+        <v>3.2974427994616438E-2</v>
       </c>
       <c r="I54" s="1">
         <f>G54/$C$7</f>
-        <v>-0.42367066895368782</v>
+        <v>0.26315789473684198</v>
       </c>
       <c r="J54" s="1">
         <f>(D54-$D$7)/$D$7</f>
@@ -1822,7 +1820,7 @@
       </c>
       <c r="K54" s="2">
         <f>(E54-$E$7)/$E$7</f>
-        <v>-0.14634146341463408</v>
+        <v>0.56249999999999989</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -1900,19 +1898,19 @@
       </c>
       <c r="F59">
         <f>B59-$B$4</f>
-        <v>-0.36999999999999922</v>
+        <v>-1.629999999999999</v>
       </c>
       <c r="G59">
         <f>C59-$C$4</f>
-        <v>-3.4400000000000004</v>
+        <v>-0.89999999999999991</v>
       </c>
       <c r="H59" s="1">
         <f>F59/$B$4</f>
-        <v>-2.8816199376946981E-2</v>
+        <v>-0.11560283687943256</v>
       </c>
       <c r="I59" s="1">
         <f>G59/$C$4</f>
-        <v>-0.73347547974413652</v>
+        <v>-0.41860465116279066</v>
       </c>
       <c r="J59" s="1">
         <f>(D59-$D$4)/$D$4</f>
@@ -1920,7 +1918,7 @@
       </c>
       <c r="K59" s="2">
         <f>(E59-$E$4)/$E$4</f>
-        <v>-0.66265060240963847</v>
+        <v>-0.39130434782608692</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -1941,19 +1939,19 @@
       </c>
       <c r="F60">
         <f>B60-$B$5</f>
-        <v>-0.98000000000000043</v>
+        <v>-2.2400000000000002</v>
       </c>
       <c r="G60">
         <f>C60-$C$5</f>
-        <v>-3.6900000000000004</v>
+        <v>-1.1499999999999999</v>
       </c>
       <c r="H60" s="1">
         <f>F60/$B$5</f>
-        <v>-7.6323987538940846E-2</v>
+        <v>-0.15886524822695036</v>
       </c>
       <c r="I60" s="1">
         <f>G60/$C$5</f>
-        <v>-0.78678038379530923</v>
+        <v>-0.53488372093023251</v>
       </c>
       <c r="J60" s="1">
         <f>(D60-$D$5)/$D$5</f>
@@ -1961,7 +1959,7 @@
       </c>
       <c r="K60" s="2">
         <f>(E60-$E$5)/$E$5</f>
-        <v>-0.72891566265060237</v>
+        <v>-0.51086956521739135</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -1982,19 +1980,19 @@
       </c>
       <c r="F61">
         <f>B61-$B$6</f>
-        <v>-0.15000000000000036</v>
+        <v>-1.58</v>
       </c>
       <c r="G61">
         <f>C61-$C$6</f>
-        <v>-3.6799999999999997</v>
+        <v>-0.78000000000000025</v>
       </c>
       <c r="H61" s="1">
         <f>F61/$B$6</f>
-        <v>-1.1424219345011451E-2</v>
+        <v>-0.10851648351648352</v>
       </c>
       <c r="I61" s="1">
         <f>G61/$C$6</f>
-        <v>-0.68785046728971966</v>
+        <v>-0.31836734693877561</v>
       </c>
       <c r="J61" s="1">
         <f>(D61-$D$6)/$D$6</f>
@@ -2002,7 +2000,7 @@
       </c>
       <c r="K61" s="2">
         <f>(E61-$E$6)/$E$6</f>
-        <v>-0.61904761904761907</v>
+        <v>-0.30769230769230776</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -2023,19 +2021,19 @@
       </c>
       <c r="F62">
         <f>B62-$B$7</f>
-        <v>6.0000000000000497E-2</v>
+        <v>-1.4699999999999989</v>
       </c>
       <c r="G62">
         <f>C62-$C$7</f>
-        <v>-3.87</v>
+        <v>-0.70000000000000018</v>
       </c>
       <c r="H62" s="1">
         <f>F62/$B$7</f>
-        <v>4.5011252813203671E-3</v>
+        <v>-9.8923283983849183E-2</v>
       </c>
       <c r="I62" s="1">
         <f>G62/$C$7</f>
-        <v>-0.66380789022298459</v>
+        <v>-0.26315789473684215</v>
       </c>
       <c r="J62" s="1">
         <f>(D62-$D$7)/$D$7</f>
@@ -2043,7 +2041,7 @@
       </c>
       <c r="K62" s="2">
         <f>(E62-$E$7)/$E$7</f>
-        <v>-0.59512195121951217</v>
+        <v>-0.25892857142857151</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -2101,19 +2099,19 @@
       </c>
       <c r="F66">
         <f>B66-$B$4</f>
-        <v>0.15000000000000036</v>
+        <v>-1.1099999999999994</v>
       </c>
       <c r="G66">
         <f>C66-$C$4</f>
-        <v>-2.5800000000000005</v>
+        <v>-4.0000000000000036E-2</v>
       </c>
       <c r="H66" s="1">
         <f>F66/$B$4</f>
-        <v>1.1682242990654233E-2</v>
+        <v>-7.872340425531911E-2</v>
       </c>
       <c r="I66" s="1">
         <f>G66/$C$4</f>
-        <v>-0.55010660980810244</v>
+        <v>-1.8604651162790715E-2</v>
       </c>
       <c r="J66" s="1">
         <f>(D66-$D$4)/$D$4</f>
@@ -2121,7 +2119,7 @@
       </c>
       <c r="K66" s="2">
         <f>(E66-$E$4)/$E$4</f>
-        <v>-0.37951807228915657</v>
+        <v>0.11956521739130432</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -2142,19 +2140,19 @@
       </c>
       <c r="F67">
         <f>B67-$B$5</f>
-        <v>-0.41000000000000014</v>
+        <v>-1.67</v>
       </c>
       <c r="G67">
         <f>C67-$C$5</f>
-        <v>-3.1800000000000006</v>
+        <v>-0.6399999999999999</v>
       </c>
       <c r="H67" s="1">
         <f>F67/$B$5</f>
-        <v>-3.1931464174454839E-2</v>
+        <v>-0.11843971631205674</v>
       </c>
       <c r="I67" s="1">
         <f>G67/$C$5</f>
-        <v>-0.67803837953091695</v>
+        <v>-0.2976744186046511</v>
       </c>
       <c r="J67" s="1">
         <f>(D67-$D$5)/$D$5</f>
@@ -2162,7 +2160,7 @@
       </c>
       <c r="K67" s="2">
         <f>(E67-$E$5)/$E$5</f>
-        <v>-0.43373493975903615</v>
+        <v>2.1739130434782507E-2</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -2183,19 +2181,19 @@
       </c>
       <c r="F68">
         <f>B68-$B$6</f>
-        <v>0.59999999999999964</v>
+        <v>-0.83000000000000007</v>
       </c>
       <c r="G68">
         <f>C68-$C$6</f>
-        <v>-2.3499999999999996</v>
+        <v>0.54999999999999982</v>
       </c>
       <c r="H68" s="1">
         <f>F68/$B$6</f>
-        <v>4.5696877380045665E-2</v>
+        <v>-5.7005494505494511E-2</v>
       </c>
       <c r="I68" s="1">
         <f>G68/$C$6</f>
-        <v>-0.43925233644859807</v>
+        <v>0.22448979591836726</v>
       </c>
       <c r="J68" s="1">
         <f>(D68-$D$6)/$D$6</f>
@@ -2203,7 +2201,7 @@
       </c>
       <c r="K68" s="2">
         <f>(E68-$E$6)/$E$6</f>
-        <v>-0.22222222222222221</v>
+        <v>0.41346153846153838</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -2224,19 +2222,19 @@
       </c>
       <c r="F69">
         <f>B69-$B$7</f>
-        <v>0.99000000000000021</v>
+        <v>-0.53999999999999915</v>
       </c>
       <c r="G69">
         <f>C69-$C$7</f>
-        <v>-2.23</v>
+        <v>0.94</v>
       </c>
       <c r="H69" s="1">
         <f>F69/$B$7</f>
-        <v>7.4268567141785466E-2</v>
+        <v>-3.6339165545087426E-2</v>
       </c>
       <c r="I69" s="1">
         <f>G69/$C$7</f>
-        <v>-0.38250428816466553</v>
+        <v>0.35338345864661652</v>
       </c>
       <c r="J69" s="1">
         <f>(D69-$D$7)/$D$7</f>
@@ -2244,7 +2242,7 @@
       </c>
       <c r="K69" s="2">
         <f>(E69-$E$7)/$E$7</f>
-        <v>-0.13658536585365846</v>
+        <v>0.58035714285714268</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -2322,19 +2320,19 @@
       </c>
       <c r="F74">
         <f>B74-$B$4</f>
-        <v>-0.35999999999999943</v>
+        <v>-1.6199999999999992</v>
       </c>
       <c r="G74">
         <f>C74-$C$4</f>
-        <v>-3.7700000000000005</v>
+        <v>-1.23</v>
       </c>
       <c r="H74" s="1">
         <f>F74/$B$4</f>
-        <v>-2.8037383177570048E-2</v>
+        <v>-0.11489361702127654</v>
       </c>
       <c r="I74" s="1">
         <f>G74/$C$4</f>
-        <v>-0.80383795309168449</v>
+        <v>-0.57209302325581401</v>
       </c>
       <c r="J74" s="1">
         <f>(D74-$D$4)/$D$4</f>
@@ -2342,7 +2340,7 @@
       </c>
       <c r="K74" s="2">
         <f>(E74-$E$4)/$E$4</f>
-        <v>-0.72891566265060237</v>
+        <v>-0.51086956521739135</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -2363,19 +2361,19 @@
       </c>
       <c r="F75">
         <f>B75-$B$5</f>
-        <v>-0.86999999999999922</v>
+        <v>-2.129999999999999</v>
       </c>
       <c r="G75">
         <f>C75-$C$5</f>
-        <v>-3.9000000000000004</v>
+        <v>-1.3599999999999999</v>
       </c>
       <c r="H75" s="1">
         <f>F75/$B$5</f>
-        <v>-6.7757009345794331E-2</v>
+        <v>-0.15106382978723398</v>
       </c>
       <c r="I75" s="1">
         <f>G75/$C$5</f>
-        <v>-0.83155650319829422</v>
+        <v>-0.63255813953488371</v>
       </c>
       <c r="J75" s="1">
         <f>(D75-$D$5)/$D$5</f>
@@ -2383,7 +2381,7 @@
       </c>
       <c r="K75" s="2">
         <f>(E75-$E$5)/$E$5</f>
-        <v>-0.7650602409638555</v>
+        <v>-0.57608695652173914</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -2404,19 +2402,19 @@
       </c>
       <c r="F76">
         <f>B76-$B$6</f>
-        <v>-0.15000000000000036</v>
+        <v>-1.58</v>
       </c>
       <c r="G76">
         <f>C76-$C$6</f>
-        <v>-4.1899999999999995</v>
+        <v>-1.2900000000000003</v>
       </c>
       <c r="H76" s="1">
         <f>F76/$B$6</f>
-        <v>-1.1424219345011451E-2</v>
+        <v>-0.10851648351648352</v>
       </c>
       <c r="I76" s="1">
         <f>G76/$C$6</f>
-        <v>-0.7831775700934579</v>
+        <v>-0.52653061224489806</v>
       </c>
       <c r="J76" s="1">
         <f>(D76-$D$6)/$D$6</f>
@@ -2424,7 +2422,7 @@
       </c>
       <c r="K76" s="2">
         <f>(E76-$E$6)/$E$6</f>
-        <v>-0.70899470899470896</v>
+        <v>-0.47115384615384615</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -2445,19 +2443,19 @@
       </c>
       <c r="F77">
         <f>B77-$B$7</f>
-        <v>2.9999999999999361E-2</v>
+        <v>-1.5</v>
       </c>
       <c r="G77">
         <f>C77-$C$7</f>
-        <v>-4.51</v>
+        <v>-1.34</v>
       </c>
       <c r="H77" s="1">
         <f>F77/$B$7</f>
-        <v>2.2505626406601172E-3</v>
+        <v>-0.1009421265141319</v>
       </c>
       <c r="I77" s="1">
         <f>G77/$C$7</f>
-        <v>-0.7735849056603773</v>
+        <v>-0.50375939849624063</v>
       </c>
       <c r="J77" s="1">
         <f>(D77-$D$7)/$D$7</f>
@@ -2465,7 +2463,7 @@
       </c>
       <c r="K77" s="2">
         <f>(E77-$E$7)/$E$7</f>
-        <v>-0.69756097560975605</v>
+        <v>-0.44642857142857151</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -2523,19 +2521,19 @@
       </c>
       <c r="F81">
         <f>B81-$B$4</f>
-        <v>0</v>
+        <v>-1.2599999999999998</v>
       </c>
       <c r="G81">
         <f>C81-$C$4</f>
-        <v>-3.2300000000000004</v>
+        <v>-0.69</v>
       </c>
       <c r="H81" s="1">
         <f>F81/$B$4</f>
-        <v>0</v>
+        <v>-8.9361702127659565E-2</v>
       </c>
       <c r="I81" s="1">
         <f>G81/$C$4</f>
-        <v>-0.68869936034115142</v>
+        <v>-0.32093023255813952</v>
       </c>
       <c r="J81" s="1">
         <f>(D81-$D$4)/$D$4</f>
@@ -2543,7 +2541,7 @@
       </c>
       <c r="K81" s="2">
         <f>(E81-$E$4)/$E$4</f>
-        <v>-0.53614457831325302</v>
+        <v>-0.1630434782608696</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -2564,19 +2562,19 @@
       </c>
       <c r="F82">
         <f>B82-$B$5</f>
-        <v>-0.49000000000000021</v>
+        <v>-1.75</v>
       </c>
       <c r="G82">
         <f>C82-$C$5</f>
-        <v>-3.5900000000000003</v>
+        <v>-1.0499999999999998</v>
       </c>
       <c r="H82" s="1">
         <f>F82/$B$5</f>
-        <v>-3.8161993769470423E-2</v>
+        <v>-0.12411347517730496</v>
       </c>
       <c r="I82" s="1">
         <f>G82/$C$5</f>
-        <v>-0.76545842217484006</v>
+        <v>-0.48837209302325574</v>
       </c>
       <c r="J82" s="1">
         <f>(D82-$D$5)/$D$5</f>
@@ -2584,7 +2582,7 @@
       </c>
       <c r="K82" s="2">
         <f>(E82-$E$5)/$E$5</f>
-        <v>-0.57831325301204817</v>
+        <v>-0.23913043478260879</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -2605,19 +2603,19 @@
       </c>
       <c r="F83">
         <f>B83-$B$6</f>
-        <v>0.37999999999999901</v>
+        <v>-1.0500000000000007</v>
       </c>
       <c r="G83">
         <f>C83-$C$6</f>
-        <v>-3.3499999999999996</v>
+        <v>-0.45000000000000018</v>
       </c>
       <c r="H83" s="1">
         <f>F83/$B$6</f>
-        <v>2.8941355674028862E-2</v>
+        <v>-7.2115384615384664E-2</v>
       </c>
       <c r="I83" s="1">
         <f>G83/$C$6</f>
-        <v>-0.62616822429906538</v>
+        <v>-0.18367346938775517</v>
       </c>
       <c r="J83" s="1">
         <f>(D83-$D$6)/$D$6</f>
@@ -2625,7 +2623,7 @@
       </c>
       <c r="K83" s="2">
         <f>(E83-$E$6)/$E$6</f>
-        <v>-0.44444444444444442</v>
+        <v>9.6153846153846229E-3</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -2646,19 +2644,19 @@
       </c>
       <c r="F84">
         <f>B84-$B$7</f>
-        <v>0.6899999999999995</v>
+        <v>-0.83999999999999986</v>
       </c>
       <c r="G84">
         <f>C84-$C$7</f>
-        <v>-3.45</v>
+        <v>-0.28000000000000025</v>
       </c>
       <c r="H84" s="1">
         <f>F84/$B$7</f>
-        <v>5.1762940735183761E-2</v>
+        <v>-5.6527590847913853E-2</v>
       </c>
       <c r="I84" s="1">
         <f>G84/$C$7</f>
-        <v>-0.59176672384219553</v>
+        <v>-0.10526315789473693</v>
       </c>
       <c r="J84" s="1">
         <f>(D84-$D$7)/$D$7</f>
@@ -2666,7 +2664,7 @@
       </c>
       <c r="K84" s="2">
         <f>(E84-$E$7)/$E$7</f>
-        <v>-0.38536585365853654</v>
+        <v>0.1249999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -2744,19 +2742,19 @@
       </c>
       <c r="F89">
         <f>B89-$B$4</f>
-        <v>-0.90000000000000036</v>
+        <v>-2.16</v>
       </c>
       <c r="G89">
         <f>C89-$C$4</f>
-        <v>-3.3900000000000006</v>
+        <v>-0.84999999999999987</v>
       </c>
       <c r="H89" s="1">
         <f>F89/$B$4</f>
-        <v>-7.0093457943925255E-2</v>
+        <v>-0.15319148936170215</v>
       </c>
       <c r="I89" s="1">
         <f>G89/$C$4</f>
-        <v>-0.72281449893390193</v>
+        <v>-0.39534883720930231</v>
       </c>
       <c r="J89" s="1">
         <f>(D89-$D$4)/$D$4</f>
@@ -2764,7 +2762,7 @@
       </c>
       <c r="K89" s="2">
         <f>(E89-$E$4)/$E$4</f>
-        <v>-0.66867469879518071</v>
+        <v>-0.40217391304347822</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -2785,19 +2783,19 @@
       </c>
       <c r="F90">
         <f>B90-$B$5</f>
-        <v>-1.3399999999999999</v>
+        <v>-2.5999999999999996</v>
       </c>
       <c r="G90">
         <f>C90-$C$5</f>
-        <v>-3.66</v>
+        <v>-1.1199999999999999</v>
       </c>
       <c r="H90" s="1">
         <f>F90/$B$5</f>
-        <v>-0.10436137071651089</v>
+        <v>-0.18439716312056736</v>
       </c>
       <c r="I90" s="1">
         <f>G90/$C$5</f>
-        <v>-0.78038379530916846</v>
+        <v>-0.52093023255813953</v>
       </c>
       <c r="J90" s="1">
         <f>(D90-$D$5)/$D$5</f>
@@ -2805,7 +2803,7 @@
       </c>
       <c r="K90" s="2">
         <f>(E90-$E$5)/$E$5</f>
-        <v>-0.74698795180722899</v>
+        <v>-0.54347826086956519</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -2826,19 +2824,19 @@
       </c>
       <c r="F91">
         <f>B91-$B$6</f>
-        <v>-0.95000000000000107</v>
+        <v>-2.3800000000000008</v>
       </c>
       <c r="G91">
         <f>C91-$C$6</f>
-        <v>-3.5999999999999996</v>
+        <v>-0.70000000000000018</v>
       </c>
       <c r="H91" s="1">
         <f>F91/$B$6</f>
-        <v>-7.2353389185072434E-2</v>
+        <v>-0.16346153846153852</v>
       </c>
       <c r="I91" s="1">
         <f>G91/$C$6</f>
-        <v>-0.67289719626168221</v>
+        <v>-0.28571428571428575</v>
       </c>
       <c r="J91" s="1">
         <f>(D91-$D$6)/$D$6</f>
@@ -2846,7 +2844,7 @@
       </c>
       <c r="K91" s="2">
         <f>(E91-$E$6)/$E$6</f>
-        <v>-0.6243386243386243</v>
+        <v>-0.31730769230769235</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -2867,19 +2865,19 @@
       </c>
       <c r="F92">
         <f>B92-$B$7</f>
-        <v>-0.91999999999999993</v>
+        <v>-2.4499999999999993</v>
       </c>
       <c r="G92">
         <f>C92-$C$7</f>
-        <v>-3.7600000000000002</v>
+        <v>-0.5900000000000003</v>
       </c>
       <c r="H92" s="1">
         <f>F92/$B$7</f>
-        <v>-6.9017254313578386E-2</v>
+        <v>-0.16487213997308206</v>
       </c>
       <c r="I92" s="1">
         <f>G92/$C$7</f>
-        <v>-0.6449399656946827</v>
+        <v>-0.22180451127819559</v>
       </c>
       <c r="J92" s="1">
         <f>(D92-$D$7)/$D$7</f>
@@ -2887,7 +2885,7 @@
       </c>
       <c r="K92" s="2">
         <f>(E92-$E$7)/$E$7</f>
-        <v>-0.60000000000000009</v>
+        <v>-0.26785714285714296</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -2945,19 +2943,19 @@
       </c>
       <c r="F96">
         <f>B96-$B$4</f>
-        <v>-0.37999999999999901</v>
+        <v>-1.6399999999999988</v>
       </c>
       <c r="G96">
         <f>C96-$C$4</f>
-        <v>-2.5000000000000004</v>
+        <v>4.0000000000000036E-2</v>
       </c>
       <c r="H96" s="1">
         <f>F96/$B$4</f>
-        <v>-2.9595015576323911E-2</v>
+        <v>-0.11631205673758857</v>
       </c>
       <c r="I96" s="1">
         <f>G96/$C$4</f>
-        <v>-0.53304904051172708</v>
+        <v>1.8604651162790715E-2</v>
       </c>
       <c r="J96" s="1">
         <f>(D96-$D$4)/$D$4</f>
@@ -2965,7 +2963,7 @@
       </c>
       <c r="K96" s="2">
         <f>(E96-$E$4)/$E$4</f>
-        <v>-0.37951807228915657</v>
+        <v>0.11956521739130432</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -2986,19 +2984,19 @@
       </c>
       <c r="F97">
         <f>B97-$B$5</f>
-        <v>-0.76999999999999957</v>
+        <v>-2.0299999999999994</v>
       </c>
       <c r="G97">
         <f>C97-$C$5</f>
-        <v>-3.1400000000000006</v>
+        <v>-0.59999999999999987</v>
       </c>
       <c r="H97" s="1">
         <f>F97/$B$5</f>
-        <v>-5.9968847352024887E-2</v>
+        <v>-0.14397163120567372</v>
       </c>
       <c r="I97" s="1">
         <f>G97/$C$5</f>
-        <v>-0.66950959488272932</v>
+        <v>-0.27906976744186041</v>
       </c>
       <c r="J97" s="1">
         <f>(D97-$D$5)/$D$5</f>
@@ -3006,7 +3004,7 @@
       </c>
       <c r="K97" s="2">
         <f>(E97-$E$5)/$E$5</f>
-        <v>-0.43373493975903615</v>
+        <v>2.1739130434782507E-2</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -3027,19 +3025,19 @@
       </c>
       <c r="F98">
         <f>B98-$B$6</f>
-        <v>-0.20000000000000107</v>
+        <v>-1.6300000000000008</v>
       </c>
       <c r="G98">
         <f>C98-$C$6</f>
-        <v>-2.2399999999999998</v>
+        <v>0.6599999999999997</v>
       </c>
       <c r="H98" s="1">
         <f>F98/$B$6</f>
-        <v>-1.5232292460015312E-2</v>
+        <v>-0.1119505494505495</v>
       </c>
       <c r="I98" s="1">
         <f>G98/$C$6</f>
-        <v>-0.4186915887850467</v>
+        <v>0.26938775510204066</v>
       </c>
       <c r="J98" s="1">
         <f>(D98-$D$6)/$D$6</f>
@@ -3047,7 +3045,7 @@
       </c>
       <c r="K98" s="2">
         <f>(E98-$E$6)/$E$6</f>
-        <v>-0.2275132275132275</v>
+        <v>0.40384615384615374</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -3068,19 +3066,19 @@
       </c>
       <c r="F99">
         <f>B99-$B$7</f>
-        <v>-9.9999999999997868E-3</v>
+        <v>-1.5399999999999991</v>
       </c>
       <c r="G99">
         <f>C99-$C$7</f>
-        <v>-2.08</v>
+        <v>1.0899999999999999</v>
       </c>
       <c r="H99" s="1">
         <f>F99/$B$7</f>
-        <v>-7.5018754688670566E-4</v>
+        <v>-0.1036339165545087</v>
       </c>
       <c r="I99" s="1">
         <f>G99/$C$7</f>
-        <v>-0.35677530017152659</v>
+        <v>0.40977443609022551</v>
       </c>
       <c r="J99" s="1">
         <f>(D99-$D$7)/$D$7</f>
@@ -3088,7 +3086,7 @@
       </c>
       <c r="K99" s="2">
         <f>(E99-$E$7)/$E$7</f>
-        <v>-0.13658536585365846</v>
+        <v>0.58035714285714268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>